<commit_message>
edited ref tables for yll
</commit_message>
<xml_diff>
--- a/tests/testthat/YLL_LE.xlsx
+++ b/tests/testthat/YLL_LE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura.Powell\Documents\projects\PHEindicatormethods_2\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32C1C0C-D6A1-4280-8A4C-911844161E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FE0FF7-39BA-4606-873E-33A18F9A58A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{FF27F328-942A-47E1-AE40-CD55D8ADFCBF}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{FF27F328-942A-47E1-AE40-CD55D8ADFCBF}"/>
   </bookViews>
   <sheets>
     <sheet name="yll_le_5yr" sheetId="1" r:id="rId1"/>
@@ -235,13 +235,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Heading 1 2" xfId="10" xr:uid="{436CEDC2-B0F0-4FD5-B5FE-54E19FE8E406}"/>
@@ -595,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6BB732-1DED-4DDE-A343-46DBACD40FBE}">
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,6 +641,9 @@
         <f>(yll_le_1yr!D2)</f>
         <v>74.5</v>
       </c>
+      <c r="E2" s="6">
+        <v>83.08</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
@@ -657,6 +661,9 @@
         <f>(yll_le_1yr!D3+yll_le_1yr!D4+yll_le_1yr!D5+yll_le_1yr!D6)/4</f>
         <v>72</v>
       </c>
+      <c r="E3" s="6">
+        <v>80.878827999999999</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
@@ -672,6 +679,9 @@
       </c>
       <c r="D4">
         <v>67.5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>76.459946000000002</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -689,6 +699,9 @@
       <c r="D5">
         <v>62.5</v>
       </c>
+      <c r="E5" s="6">
+        <v>71.505289000000005</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
@@ -705,6 +718,9 @@
       <c r="D6">
         <v>57.5</v>
       </c>
+      <c r="E6" s="6">
+        <v>66.434832</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
@@ -721,6 +737,9 @@
       <c r="D7">
         <v>52.5</v>
       </c>
+      <c r="E7" s="6">
+        <v>61.488934999999998</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
@@ -737,6 +756,9 @@
       <c r="D8">
         <v>47.5</v>
       </c>
+      <c r="E8" s="6">
+        <v>56.616292000000001</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
@@ -753,6 +775,9 @@
       <c r="D9">
         <v>42.5</v>
       </c>
+      <c r="E9" s="6">
+        <v>51.724936999999997</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
@@ -769,6 +794,9 @@
       <c r="D10">
         <v>37.5</v>
       </c>
+      <c r="E10" s="6">
+        <v>46.916581999999998</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
@@ -785,6 +813,9 @@
       <c r="D11">
         <v>32.5</v>
       </c>
+      <c r="E11" s="6">
+        <v>41.956308</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
@@ -801,6 +832,9 @@
       <c r="D12">
         <v>27.5</v>
       </c>
+      <c r="E12" s="6">
+        <v>37.257553000000001</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
@@ -817,6 +851,9 @@
       <c r="D13">
         <v>22.5</v>
       </c>
+      <c r="E13" s="6">
+        <v>32.619971999999997</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
@@ -833,6 +870,9 @@
       <c r="D14">
         <v>17.5</v>
       </c>
+      <c r="E14" s="6">
+        <v>28.101426</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
@@ -849,6 +889,9 @@
       <c r="D15">
         <v>12.5</v>
       </c>
+      <c r="E15" s="6">
+        <v>23.678177000000002</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
@@ -865,6 +908,9 @@
       <c r="D16">
         <v>7.5</v>
       </c>
+      <c r="E16" s="6">
+        <v>19.365911000000001</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
@@ -881,6 +927,9 @@
       <c r="D17">
         <v>2.5</v>
       </c>
+      <c r="E17" s="6">
+        <v>15.514853</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
@@ -897,6 +946,9 @@
       <c r="D18">
         <v>0</v>
       </c>
+      <c r="E18" s="6">
+        <v>11.792838</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
@@ -913,6 +965,9 @@
       <c r="D19">
         <v>0</v>
       </c>
+      <c r="E19" s="6">
+        <v>8.6029809999999998</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
@@ -929,6 +984,9 @@
       <c r="D20">
         <v>0</v>
       </c>
+      <c r="E20" s="6">
+        <v>6.0185110000000002</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
@@ -945,6 +1003,9 @@
       <c r="D21">
         <v>0</v>
       </c>
+      <c r="E21" s="6">
+        <v>3.7965770000000001</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
@@ -960,6 +1021,9 @@
       </c>
       <c r="D22">
         <v>74.5</v>
+      </c>
+      <c r="E22" s="6">
+        <v>79.459999999999994</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -977,6 +1041,9 @@
       <c r="D23">
         <v>72</v>
       </c>
+      <c r="E23" s="6">
+        <v>77.300284000000005</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
@@ -992,6 +1059,9 @@
       </c>
       <c r="D24">
         <v>67.5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>72.877994999999999</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1009,6 +1079,9 @@
       <c r="D25">
         <v>62.5</v>
       </c>
+      <c r="E25" s="6">
+        <v>67.925471999999999</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
@@ -1025,6 +1098,9 @@
       <c r="D26">
         <v>57.5</v>
       </c>
+      <c r="E26" s="6">
+        <v>62.865049999999997</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
@@ -1041,6 +1117,9 @@
       <c r="D27">
         <v>52.5</v>
       </c>
+      <c r="E27" s="6">
+        <v>58.021082999999997</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
@@ -1057,6 +1136,9 @@
       <c r="D28">
         <v>47.5</v>
       </c>
+      <c r="E28" s="6">
+        <v>53.213501999999998</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
@@ -1073,6 +1155,9 @@
       <c r="D29">
         <v>42.5</v>
       </c>
+      <c r="E29" s="6">
+        <v>48.387422999999998</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
@@ -1089,6 +1174,9 @@
       <c r="D30">
         <v>37.5</v>
       </c>
+      <c r="E30" s="6">
+        <v>43.655194000000002</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
@@ -1105,6 +1193,9 @@
       <c r="D31">
         <v>32.5</v>
       </c>
+      <c r="E31" s="6">
+        <v>38.802669999999999</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
@@ -1121,6 +1212,9 @@
       <c r="D32">
         <v>27.5</v>
       </c>
+      <c r="E32" s="6">
+        <v>34.210920000000002</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
@@ -1137,6 +1231,9 @@
       <c r="D33">
         <v>22.5</v>
       </c>
+      <c r="E33" s="6">
+        <v>29.710315000000001</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
@@ -1153,6 +1250,9 @@
       <c r="D34">
         <v>17.5</v>
       </c>
+      <c r="E34" s="6">
+        <v>25.336711000000001</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
@@ -1169,6 +1269,9 @@
       <c r="D35">
         <v>12.5</v>
       </c>
+      <c r="E35" s="6">
+        <v>21.12154</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
@@ -1185,6 +1288,9 @@
       <c r="D36">
         <v>7.5</v>
       </c>
+      <c r="E36" s="6">
+        <v>17.085767000000001</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
@@ -1201,6 +1307,9 @@
       <c r="D37">
         <v>2.5</v>
       </c>
+      <c r="E37" s="6">
+        <v>13.550349000000001</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
@@ -1217,6 +1326,9 @@
       <c r="D38">
         <v>0</v>
       </c>
+      <c r="E38" s="6">
+        <v>10.199809999999999</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
@@ -1233,6 +1345,9 @@
       <c r="D39">
         <v>0</v>
       </c>
+      <c r="E39" s="6">
+        <v>7.4235429999999996</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
@@ -1249,6 +1364,9 @@
       <c r="D40">
         <v>0</v>
       </c>
+      <c r="E40" s="6">
+        <v>5.2128209999999999</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
     </row>
@@ -1264,6 +1382,9 @@
       </c>
       <c r="D41">
         <v>0</v>
+      </c>
+      <c r="E41" s="6">
+        <v>3.4080970000000002</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -2251,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A16C59A-5FC6-41A4-8E22-DC77818FC60E}">
   <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
YLL LE using ONS life tables for 5 year age bands
</commit_message>
<xml_diff>
--- a/tests/testthat/YLL_LE.xlsx
+++ b/tests/testthat/YLL_LE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura.Powell\Documents\projects\PHEindicatormethods_2\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FE0FF7-39BA-4606-873E-33A18F9A58A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656BE420-0BCB-40EB-8879-EC567717B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{FF27F328-942A-47E1-AE40-CD55D8ADFCBF}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,16 +167,306 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -211,8 +501,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -234,6 +604,47 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -244,17 +655,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="59">
+    <cellStyle name="20% - Accent1" xfId="36" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="40" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="44" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="48" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="52" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="56" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="37" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="41" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="45" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="49" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="53" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="57" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="38" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="42" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="50" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="54" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="58" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="35" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="39" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="43" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="47" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="51" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="55" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="24" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="28" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="30" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="33" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="23" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="19" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="10" xr:uid="{436CEDC2-B0F0-4FD5-B5FE-54E19FE8E406}"/>
     <cellStyle name="Heading 1 3" xfId="2" xr:uid="{34B4E97D-BCB4-4696-A014-C142498A501A}"/>
+    <cellStyle name="Heading 2" xfId="20" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 2 2" xfId="3" xr:uid="{6378093F-85AA-45B0-8CE9-8369B503F698}"/>
+    <cellStyle name="Heading 3" xfId="21" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 3 2" xfId="12" xr:uid="{19C10A59-8A70-4F14-9A7D-4CE830071BF2}"/>
+    <cellStyle name="Heading 4" xfId="22" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{20EECFCB-0803-4A54-BE00-C63A4DF0DA34}"/>
     <cellStyle name="Hyperlink 2 2" xfId="6" xr:uid="{68DB300E-0733-4047-B783-0C78EC53BC3B}"/>
     <cellStyle name="Hyperlink 2 3" xfId="17" xr:uid="{636CCCC6-E606-4494-A170-24794E566B10}"/>
     <cellStyle name="Hyperlink 2 4" xfId="14" xr:uid="{561516DE-6B01-4412-B892-F0740CBE75F1}"/>
     <cellStyle name="Hyperlink 3" xfId="7" xr:uid="{A3D9E670-8654-4532-84DD-C9E6471F9C9C}"/>
     <cellStyle name="Hyperlink 4" xfId="13" xr:uid="{7D2E235A-B9A8-4835-BD5A-B6A601DCE0B4}"/>
+    <cellStyle name="Input" xfId="26" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="29" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="25" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{8853A671-B717-46D4-8194-BC9855C5ECD3}"/>
     <cellStyle name="Normal 2 2" xfId="9" xr:uid="{18BF7486-D5C6-4A94-807E-1983AFE591A3}"/>
@@ -263,6 +710,11 @@
     <cellStyle name="Normal 4" xfId="1" xr:uid="{C8F8789E-151D-4EA6-9FB0-71A0430767AD}"/>
     <cellStyle name="Normal 5" xfId="16" xr:uid="{DC31FDCE-B400-4530-910C-EB2F4DF95CBA}"/>
     <cellStyle name="Normal 6" xfId="11" xr:uid="{176AD5D8-EF13-4E80-A9D4-1F7D82AED38A}"/>
+    <cellStyle name="Note" xfId="32" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="27" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="18" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="34" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="31" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,7 +1049,7 @@
   <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E41"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,7 +1086,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>83.05</v>
       </c>
       <c r="D2">
@@ -642,9 +1094,9 @@
         <v>74.5</v>
       </c>
       <c r="E2" s="6">
-        <v>83.08</v>
-      </c>
-      <c r="G2" s="5"/>
+        <v>83.18</v>
+      </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8">
@@ -654,7 +1106,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>82.34</v>
       </c>
       <c r="D3">
@@ -662,9 +1114,9 @@
         <v>72</v>
       </c>
       <c r="E3" s="6">
-        <v>80.878827999999999</v>
-      </c>
-      <c r="G3" s="5"/>
+        <v>80.986740999999995</v>
+      </c>
+      <c r="G3" s="6"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8">
@@ -674,16 +1126,16 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>78.38</v>
       </c>
       <c r="D4">
         <v>67.5</v>
       </c>
       <c r="E4" s="6">
-        <v>76.459946000000002</v>
-      </c>
-      <c r="G4" s="5"/>
+        <v>76.520178999999999</v>
+      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8">
@@ -693,16 +1145,16 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>73.41</v>
       </c>
       <c r="D5">
         <v>62.5</v>
       </c>
       <c r="E5" s="6">
-        <v>71.505289000000005</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>71.566869999999994</v>
+      </c>
+      <c r="G5" s="6"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8">
@@ -712,16 +1164,16 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>68.430000000000007</v>
       </c>
       <c r="D6">
         <v>57.5</v>
       </c>
       <c r="E6" s="6">
-        <v>66.434832</v>
-      </c>
-      <c r="G6" s="5"/>
+        <v>66.628975999999994</v>
+      </c>
+      <c r="G6" s="6"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8">
@@ -731,16 +1183,16 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>63.48</v>
       </c>
       <c r="D7">
         <v>52.5</v>
       </c>
       <c r="E7" s="6">
-        <v>61.488934999999998</v>
-      </c>
-      <c r="G7" s="5"/>
+        <v>61.612335000000002</v>
+      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8">
@@ -750,16 +1202,16 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>58.55</v>
       </c>
       <c r="D8">
         <v>47.5</v>
       </c>
       <c r="E8" s="6">
-        <v>56.616292000000001</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>56.705190000000002</v>
+      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8">
@@ -769,16 +1221,16 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>53.63</v>
       </c>
       <c r="D9">
         <v>42.5</v>
       </c>
       <c r="E9" s="6">
-        <v>51.724936999999997</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>51.803880999999997</v>
+      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8">
@@ -788,16 +1240,16 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>48.74</v>
       </c>
       <c r="D10">
         <v>37.5</v>
       </c>
       <c r="E10" s="6">
-        <v>46.916581999999998</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>46.984133</v>
+      </c>
+      <c r="G10" s="6"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8">
@@ -807,16 +1259,16 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>43.91</v>
       </c>
       <c r="D11">
         <v>32.5</v>
       </c>
       <c r="E11" s="6">
-        <v>41.956308</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>42.161216000000003</v>
+      </c>
+      <c r="G11" s="6"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8">
@@ -826,16 +1278,16 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>39.14</v>
       </c>
       <c r="D12">
         <v>27.5</v>
       </c>
       <c r="E12" s="6">
-        <v>37.257553000000001</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>37.386864000000003</v>
+      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8">
@@ -845,16 +1297,16 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>34.46</v>
       </c>
       <c r="D13">
         <v>22.5</v>
       </c>
       <c r="E13" s="6">
-        <v>32.619971999999997</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>32.735224000000002</v>
+      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8">
@@ -864,16 +1316,16 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>29.89</v>
       </c>
       <c r="D14">
         <v>17.5</v>
       </c>
       <c r="E14" s="6">
-        <v>28.101426</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>28.229182000000002</v>
+      </c>
+      <c r="G14" s="6"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8">
@@ -883,16 +1335,16 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>25.43</v>
       </c>
       <c r="D15">
         <v>12.5</v>
       </c>
       <c r="E15" s="6">
-        <v>23.678177000000002</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>23.880032</v>
+      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8">
@@ -902,16 +1354,16 @@
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>21.14</v>
       </c>
       <c r="D16">
         <v>7.5</v>
       </c>
       <c r="E16" s="6">
-        <v>19.365911000000001</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>19.653469999999999</v>
+      </c>
+      <c r="G16" s="6"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8">
@@ -921,16 +1373,16 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>17.07</v>
       </c>
       <c r="D17">
         <v>2.5</v>
       </c>
       <c r="E17" s="6">
-        <v>15.514853</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>15.608923000000001</v>
+      </c>
+      <c r="G17" s="6"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8">
@@ -940,16 +1392,16 @@
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>13.26</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" s="6">
-        <v>11.792838</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>12.015802000000001</v>
+      </c>
+      <c r="G18" s="6"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8">
@@ -959,16 +1411,16 @@
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>9.7899999999999991</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" s="6">
-        <v>8.6029809999999998</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>8.7031089999999995</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8">
@@ -978,16 +1430,16 @@
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>6.9</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" s="6">
-        <v>6.0185110000000002</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>6.0398820000000004</v>
+      </c>
+      <c r="G20" s="6"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8">
@@ -997,16 +1449,16 @@
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>4.6500000000000004</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" s="6">
-        <v>3.7965770000000001</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>3.7104900000000001</v>
+      </c>
+      <c r="G21" s="6"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8">
@@ -1016,16 +1468,16 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>79.11</v>
       </c>
       <c r="D22">
         <v>74.5</v>
       </c>
       <c r="E22" s="6">
-        <v>79.459999999999994</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>79.239999999999995</v>
+      </c>
+      <c r="G22" s="6"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8">
@@ -1035,16 +1487,16 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>78.47</v>
       </c>
       <c r="D23">
         <v>72</v>
       </c>
       <c r="E23" s="6">
-        <v>77.300284000000005</v>
-      </c>
-      <c r="G23" s="5"/>
+        <v>77.125911000000002</v>
+      </c>
+      <c r="G23" s="6"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8">
@@ -1054,16 +1506,16 @@
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>74.510000000000005</v>
       </c>
       <c r="D24">
         <v>67.5</v>
       </c>
       <c r="E24" s="6">
-        <v>72.877994999999999</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>72.66431</v>
+      </c>
+      <c r="G24" s="6"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8">
@@ -1073,16 +1525,16 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>69.540000000000006</v>
       </c>
       <c r="D25">
         <v>62.5</v>
       </c>
       <c r="E25" s="6">
-        <v>67.925471999999999</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>67.716920000000002</v>
+      </c>
+      <c r="G25" s="6"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8">
@@ -1092,16 +1544,16 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>64.569999999999993</v>
       </c>
       <c r="D26">
         <v>57.5</v>
       </c>
       <c r="E26" s="6">
-        <v>62.865049999999997</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>62.791722</v>
+      </c>
+      <c r="G26" s="6"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8">
@@ -1111,16 +1563,16 @@
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>59.67</v>
       </c>
       <c r="D27">
         <v>52.5</v>
       </c>
       <c r="E27" s="6">
-        <v>58.021082999999997</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>57.875101000000001</v>
+      </c>
+      <c r="G27" s="6"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8">
@@ -1130,16 +1582,16 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>54.82</v>
       </c>
       <c r="D28">
         <v>47.5</v>
       </c>
       <c r="E28" s="6">
-        <v>53.213501999999998</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>53.041542</v>
+      </c>
+      <c r="G28" s="6"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8">
@@ -1149,16 +1601,16 @@
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>49.98</v>
       </c>
       <c r="D29">
         <v>42.5</v>
       </c>
       <c r="E29" s="6">
-        <v>48.387422999999998</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>48.219574999999999</v>
+      </c>
+      <c r="G29" s="6"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8">
@@ -1168,16 +1620,16 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>45.19</v>
       </c>
       <c r="D30">
         <v>37.5</v>
       </c>
       <c r="E30" s="6">
-        <v>43.655194000000002</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>43.48668</v>
+      </c>
+      <c r="G30" s="6"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8">
@@ -1187,16 +1639,16 @@
       <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>40.46</v>
       </c>
       <c r="D31">
         <v>32.5</v>
       </c>
       <c r="E31" s="6">
-        <v>38.802669999999999</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>38.777555999999997</v>
+      </c>
+      <c r="G31" s="6"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8">
@@ -1206,16 +1658,16 @@
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>35.82</v>
       </c>
       <c r="D32">
         <v>27.5</v>
       </c>
       <c r="E32" s="6">
-        <v>34.210920000000002</v>
-      </c>
-      <c r="G32" s="5"/>
+        <v>34.144305000000003</v>
+      </c>
+      <c r="G32" s="6"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8">
@@ -1225,16 +1677,16 @@
       <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>31.29</v>
       </c>
       <c r="D33">
         <v>22.5</v>
       </c>
       <c r="E33" s="6">
-        <v>29.710315000000001</v>
-      </c>
-      <c r="G33" s="5"/>
+        <v>29.660077999999999</v>
+      </c>
+      <c r="G33" s="6"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8">
@@ -1244,16 +1696,16 @@
       <c r="B34" t="s">
         <v>4</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>26.91</v>
       </c>
       <c r="D34">
         <v>17.5</v>
       </c>
       <c r="E34" s="6">
-        <v>25.336711000000001</v>
-      </c>
-      <c r="G34" s="5"/>
+        <v>25.360189999999999</v>
+      </c>
+      <c r="G34" s="6"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8">
@@ -1263,16 +1715,16 @@
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>22.68</v>
       </c>
       <c r="D35">
         <v>12.5</v>
       </c>
       <c r="E35" s="6">
-        <v>21.12154</v>
-      </c>
-      <c r="G35" s="5"/>
+        <v>21.245259999999998</v>
+      </c>
+      <c r="G35" s="6"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8">
@@ -1282,16 +1734,16 @@
       <c r="B36" t="s">
         <v>4</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>18.670000000000002</v>
       </c>
       <c r="D36">
         <v>7.5</v>
       </c>
       <c r="E36" s="6">
-        <v>17.085767000000001</v>
-      </c>
-      <c r="G36" s="5"/>
+        <v>17.312225000000002</v>
+      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8">
@@ -1301,16 +1753,16 @@
       <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>14.93</v>
       </c>
       <c r="D37">
         <v>2.5</v>
       </c>
       <c r="E37" s="6">
-        <v>13.550349000000001</v>
-      </c>
-      <c r="G37" s="5"/>
+        <v>13.621286</v>
+      </c>
+      <c r="G37" s="6"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8">
@@ -1320,16 +1772,16 @@
       <c r="B38" t="s">
         <v>4</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>11.5</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38" s="6">
-        <v>10.199809999999999</v>
-      </c>
-      <c r="G38" s="5"/>
+        <v>10.400986</v>
+      </c>
+      <c r="G38" s="6"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8">
@@ -1339,16 +1791,16 @@
       <c r="B39" t="s">
         <v>4</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>8.42</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" s="6">
-        <v>7.4235429999999996</v>
-      </c>
-      <c r="G39" s="5"/>
+        <v>7.482259</v>
+      </c>
+      <c r="G39" s="6"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8">
@@ -1358,16 +1810,16 @@
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>5.93</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40" s="6">
-        <v>5.2128209999999999</v>
-      </c>
-      <c r="G40" s="5"/>
+        <v>5.1860520000000001</v>
+      </c>
+      <c r="G40" s="6"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8">
@@ -1377,16 +1829,16 @@
       <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>4.01</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41" s="6">
-        <v>3.4080970000000002</v>
-      </c>
-      <c r="G41" s="5"/>
+        <v>3.302702</v>
+      </c>
+      <c r="G41" s="6"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" ht="15.75">

</xml_diff>